<commit_message>
DataBlockDescription builder API part 11 - Documentation
Former-commit-id: 895dc05a4436f76bc578656230d359f4bfb51f0b
</commit_message>
<xml_diff>
--- a/jMetaDocs/DesignConcept/FeaturesFormate.xlsx
+++ b/jMetaDocs/DesignConcept/FeaturesFormate.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programmieren\01_Java\02_projects\jMeta\trunk\jMetaDocs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programmieren\01_Java\02_projects\jMeta\trunk\jMetaDocs\DesignConcept\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="352" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="352"/>
   </bookViews>
   <sheets>
     <sheet name="MultimediaContainers" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1">MetadataContainers!$A$2:$I$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0">MultimediaContainers!$A$2:$F$2</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="91">
   <si>
     <t>APEv1</t>
   </si>
@@ -295,12 +295,36 @@
   </si>
   <si>
     <t>Tag, allows hierarchical nesting; attributes are containers called user comments</t>
+  </si>
+  <si>
+    <t>Field Types</t>
+  </si>
+  <si>
+    <t>String and "Enumerated" (Genre)</t>
+  </si>
+  <si>
+    <t>String, binary, flags, numeric and "Enumerated" (Text encoding)</t>
+  </si>
+  <si>
+    <t>String, binary, flags, numeric, "Enumerated" (Text encoding), and String List</t>
+  </si>
+  <si>
+    <t>String, binary, flags, numeric</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>String, binary, numeric</t>
+  </si>
+  <si>
+    <t>String, binary, numeric, flags</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -368,8 +392,36 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -678,13 +730,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="B5:F5"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,6 +908,26 @@
         <v>69</v>
       </c>
     </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:F2"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -865,13 +937,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1173,6 +1245,35 @@
         <v>27</v>
       </c>
     </row>
+    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:I2"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>